<commit_message>
Made slight additions to ObservationProbes table
</commit_message>
<xml_diff>
--- a/docs/ObservationalProbes.xlsx
+++ b/docs/ObservationalProbes.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawson/Git/specialdark/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="0" windowWidth="25780" windowHeight="19940" tabRatio="500"/>
+    <workbookView xWindow="2120" yWindow="460" windowWidth="25780" windowHeight="19940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +23,62 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Will Dawson</author>
+  </authors>
+  <commentList>
+    <comment ref="A27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Will Dawson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+What does EoR mean?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Will Dawson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+What does CBR mean?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>Small scale structure</t>
   </si>
@@ -160,9 +219,6 @@
   </si>
   <si>
     <t>Weak lensing stacks</t>
-  </si>
-  <si>
-    <t>Strong+weak lensing</t>
   </si>
   <si>
     <t>Galaxy-cluster mergers</t>
@@ -213,20 +269,23 @@
 Power in potential fluctuations</t>
   </si>
   <si>
-    <t>SDSS, DES, GAIA, WFIRST</t>
-  </si>
-  <si>
     <t>Presently productive</t>
   </si>
   <si>
     <t>Future potential</t>
+  </si>
+  <si>
+    <t>Spectroscopy, Strong+weak lensing</t>
+  </si>
+  <si>
+    <t>SDSS, DES, GAIA, LSST, WFIRST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -270,6 +329,24 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -446,76 +523,77 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -548,6 +626,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -872,14 +955,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="Z4" sqref="Z4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="AD34" sqref="AD34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
@@ -891,163 +974,163 @@
     <col min="27" max="28" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
-      <c r="D1" s="18" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="D1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-    </row>
-    <row r="2" spans="1:28" ht="148" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+    </row>
+    <row r="2" spans="1:28" ht="148" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="22" t="s">
+      <c r="J2" s="18"/>
+      <c r="K2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="17"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA2" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" s="14"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="101" customHeight="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="7" t="s">
+      <c r="AB2" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="101" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="15" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="R3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="S3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="17" t="s">
+      <c r="T3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="U3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="V3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W3" s="17" t="s">
+      <c r="W3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="X3" s="17" t="s">
+      <c r="X3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="Y3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-    </row>
-    <row r="5" spans="1:28">
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1055,12 +1138,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1068,81 +1151,81 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
-    </row>
-    <row r="10" spans="1:28">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="V11" s="23"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="V11" s="9"/>
       <c r="Z11" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="23"/>
-    </row>
-    <row r="12" spans="1:28">
+        <v>65</v>
+      </c>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1150,7 +1233,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1158,7 +1241,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1166,7 +1249,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1174,23 +1257,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1198,7 +1281,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1206,61 +1289,87 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>44</v>
       </c>
       <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="T24" s="9"/>
+      <c r="AB24" s="9"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="9"/>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="9"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>51</v>
       </c>
-      <c r="B28" t="s">
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="B29" t="s">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>54</v>
       </c>
       <c r="B30" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
         <v>59</v>
-      </c>
-      <c r="B31" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1270,6 +1379,7 @@
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="AB2:AB3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:Y1"/>
     <mergeCell ref="K2:N2"/>
@@ -1278,14 +1388,9 @@
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="D2:F2"/>
-    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>